<commit_message>
Removed manual roster and changed roster dict to include a nested dict with bible study data
</commit_message>
<xml_diff>
--- a/formats/bstud_format_download.xlsx
+++ b/formats/bstud_format_download.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Desktop/getto_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06881278-7D73-774C-AEC5-7E2CEEB2BF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EC980B-1B55-0A48-9CB9-3201238F7D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="11340" windowHeight="11420" xr2:uid="{8BA19672-DC71-F541-B880-63FA370FFD8F}"/>
   </bookViews>
@@ -38,21 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
-    <t>Monday 1600-1700</t>
-  </si>
-  <si>
-    <t>Tuesday 1600-1700</t>
-  </si>
-  <si>
-    <t>Wednesday 1600-1700</t>
-  </si>
-  <si>
-    <t>Thursday 1600-1700</t>
-  </si>
-  <si>
-    <t>Friday 1600-1700</t>
-  </si>
-  <si>
     <t>Nono</t>
   </si>
   <si>
@@ -174,6 +159,21 @@
   </si>
   <si>
     <t>Tross</t>
+  </si>
+  <si>
+    <t>Monday 1600</t>
+  </si>
+  <si>
+    <t>Tuesday 1600</t>
+  </si>
+  <si>
+    <t>Wednesday 1600</t>
+  </si>
+  <si>
+    <t>Thursday 1600</t>
+  </si>
+  <si>
+    <t>Friday 1600</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,160 +575,160 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>